<commit_message>
added excel to leo
</commit_message>
<xml_diff>
--- a/Leo.xlsx
+++ b/Leo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nage\Robot clones\RobotFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF615D14-CA8B-46C0-9C4F-544E6638BEA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87594EBD-632D-46F2-9D91-24A5093FAD55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{84BA3C9F-EB62-4C7C-BFE2-9D31F26210F9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>id</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>NOTVALID2</t>
+  </si>
+  <si>
+    <t>Hallo</t>
   </si>
 </sst>
 </file>
@@ -394,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774ACF65-26BD-4B5B-B01B-7AA6A158F72D}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,6 +453,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
xlsx check lists added
</commit_message>
<xml_diff>
--- a/Leo.xlsx
+++ b/Leo.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nage\Robot clones\RobotFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87594EBD-632D-46F2-9D91-24A5093FAD55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C79056-BA8E-425A-AF4A-F3DE3E258C8D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{84BA3C9F-EB62-4C7C-BFE2-9D31F26210F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -400,7 +401,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,4 +465,22 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5FDC95-04A8-4014-AFA6-E377F2CEA7DE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>